<commit_message>
add some empty file
</commit_message>
<xml_diff>
--- a/Assets/Data/ChapterScriptConfig.xlsx
+++ b/Assets/Data/ChapterScriptConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\FinalProject\Assets\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10545\Desktop\FinalProject\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB60A024-A6D2-40D8-9EAB-643BC8017D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25C0921-B850-4366-8A9F-5C4201914F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5670" yWindow="1950" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +36,126 @@
   </si>
   <si>
     <t>JiYouPaiFang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WoLunZengYa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JiyouLengQue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JieQiMenTi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JinQiQiGuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RanYouPenShe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChuShuiKou</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZhenKongBeng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DianHuoXianQuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RanYouDaoGui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TuLunZhouGai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PeiQiZhengShi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NiuZhuanJianZhen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FaDongJiQianGai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZhengShiLian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TuLunZhouZhengShiChiLun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JinQiTuLunZhou</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PaiQiTuLunZhou</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QiMenYaoBi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JianXiTiaoJieQi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QiGangGai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YouDiKe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JiYouBengChuanDongLianTiao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JiYouBeng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JiYouDaoLiuBan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LianGanZhouChengGai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HuoSaiLianGan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QiHuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YouHuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XiaBuQuZhouXiang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuZhou</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -361,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -388,6 +508,246 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>201</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>202</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>203</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>204</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>205</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>206</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>301</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>302</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>303</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>304</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>401</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>501</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>502</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>503</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>504</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>601</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>602</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>603</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>604</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>701</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>702</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>